<commit_message>
Update SEC-specs and costings.xlsx
</commit_message>
<xml_diff>
--- a/SEC-specs and costings.xlsx
+++ b/SEC-specs and costings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B\Dropbox\open source code\specs and costings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benj\Dropbox\open source code\specs and costings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762D2206-DB51-4B17-818A-515F1F053B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91231708-5235-4E5B-83F5-B0ECFD777B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="4900" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="high throughput, iDus + Autolab" sheetId="2" r:id="rId1"/>
+    <sheet name="AutoLab + ocean optics" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>Description</t>
   </si>
@@ -295,13 +296,55 @@
   </si>
   <si>
     <t>TOTALS:</t>
+  </si>
+  <si>
+    <t>CALL AND DISCUSS COMPATIBILIY WITH SUPPLIERs BEFORE PURCHASING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIS LIST IS INTENDED AS A GUIDE ONLY </t>
+  </si>
+  <si>
+    <t>CALL THE SUPPLIERS AND DISCUSS COMPATIBILIY WITH  BEFORE PURCHASING</t>
+  </si>
+  <si>
+    <t>I bought  high post holders but consider getting smaller ones - the referance electrode+ cell tends to be too high to close the enclosure</t>
+  </si>
+  <si>
+    <t>XE25C11D/M - 525 mm x 375 mm x 300 mm (L x W x H) Aluminum Enclosure with Hinged L-Shaped Door </t>
+  </si>
+  <si>
+    <t>XE25C11D/M</t>
+  </si>
+  <si>
+    <t>https://www.thorlabs.com/thorproduct.cfm?partnumber=XE25C11D/M</t>
+  </si>
+  <si>
+    <t>UV/VIS Collimating Lens, 200-2500 nm</t>
+  </si>
+  <si>
+    <t>600 um Premium Fiber, VIS/NIR, 1 m</t>
+  </si>
+  <si>
+    <t>From ocean optics</t>
+  </si>
+  <si>
+    <t>Total components</t>
+  </si>
+  <si>
+    <t>Check that these legs are compatible with the thorlabs source and they  all come to the correct height I used spare legs from our lab</t>
+  </si>
+  <si>
+    <t>Note: we use ocean optics' light soutce which is not very good. I have updated this list with a thorlabs source but please check compatiability</t>
+  </si>
+  <si>
+    <t>Get size that suits your space requirments the thorlabs light source is long so these could get in the way of each other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
       <color theme="1"/>
@@ -378,8 +421,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,8 +494,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -475,13 +565,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -493,9 +592,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -537,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -545,7 +644,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -558,7 +657,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -568,6 +667,18 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -890,404 +1001,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="26" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
-    <col min="3" max="3" width="14.546875" customWidth="1"/>
-    <col min="4" max="4" width="4.34765625" customWidth="1"/>
-    <col min="5" max="5" width="7.34765625" customWidth="1"/>
-    <col min="6" max="6" width="21.3984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="39.84765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.78515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.35546875" customWidth="1"/>
+    <col min="5" max="5" width="7.35546875" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="183.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C3" s="10">
         <v>5212.88</v>
       </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
         <v>5212.88</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A3" s="12" t="s">
+    <row r="4" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C4" s="8">
         <v>350.46</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D4" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="8">
-        <f t="shared" ref="E3" si="0">C3*D3</f>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4" si="0">C4*D4</f>
         <v>700.92</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A4" s="12"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="12"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C6" s="13">
         <v>72.89</v>
-      </c>
-      <c r="D5" s="13">
-        <v>3</v>
-      </c>
-      <c r="E5" s="13">
-        <f>C5*D5</f>
-        <v>218.67000000000002</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="13">
-        <v>46.75</v>
       </c>
       <c r="D6" s="13">
         <v>3</v>
       </c>
       <c r="E6" s="13">
-        <f t="shared" ref="E6:E9" si="1">C6*D6</f>
+        <f>C6*D6</f>
+        <v>218.67000000000002</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="13">
+        <v>46.75</v>
+      </c>
+      <c r="D7" s="13">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" ref="E7:E10" si="1">C7*D7</f>
         <v>140.25</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C8" s="8">
         <v>12.96</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D8" s="8">
         <v>8</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E8" s="8">
         <f t="shared" si="1"/>
         <v>103.68</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C9" s="13">
         <v>9.7799999999999994</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D9" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E9" s="13">
         <f t="shared" si="1"/>
         <v>78.239999999999995</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="104" x14ac:dyDescent="0.6">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.4">
+      <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C10" s="8">
         <v>171.81</v>
       </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
         <f t="shared" si="1"/>
         <v>171.81</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="104" x14ac:dyDescent="0.6">
-      <c r="A10" s="12" t="s">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.4">
+      <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C11" s="13">
         <v>43.78</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D11" s="13">
         <v>4</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E11" s="13">
         <v>146.19999999999999</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="78" x14ac:dyDescent="0.6">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C12" s="8">
         <v>4</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="8">
         <v>13.18</v>
       </c>
-      <c r="E11" s="8">
-        <f t="shared" ref="E11:E16" si="2">C11*D11</f>
+      <c r="E12" s="8">
+        <f t="shared" ref="E12:E17" si="2">C12*D12</f>
         <v>52.72</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="104" x14ac:dyDescent="0.6">
-      <c r="A12" s="17" t="s">
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.4">
+      <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="8">
         <v>81.680000000000007</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E13" s="8">
         <f t="shared" si="2"/>
         <v>163.36000000000001</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="72.5" x14ac:dyDescent="0.6">
-      <c r="A13" s="12" t="s">
+    <row r="14" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C14" s="8">
         <v>197.2</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <v>2</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E14" s="8">
         <f t="shared" si="2"/>
         <v>394.4</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.6">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:7" ht="74.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C15" s="8">
         <v>840.2</v>
       </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
         <f t="shared" si="2"/>
         <v>840.2</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C16" s="8">
         <v>153.07</v>
       </c>
-      <c r="D15" s="8">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
         <f t="shared" si="2"/>
         <v>153.07</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="37.5" x14ac:dyDescent="0.6">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.4">
+      <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C17" s="45">
         <v>83.25</v>
       </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
         <f t="shared" si="2"/>
         <v>83.25</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.6">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.4">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C18" s="19">
         <v>5086</v>
       </c>
-      <c r="D17" s="19">
-        <v>1</v>
-      </c>
-      <c r="E17" s="19">
-        <f>C17*D17</f>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <f t="shared" ref="E18:E26" si="3">C18*D18</f>
         <v>5086</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A18" s="18" t="s">
+    <row r="19" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B19" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="19">
-        <v>666</v>
-      </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="19">
-        <f>C18*D18</f>
-        <v>666</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="55" x14ac:dyDescent="0.6">
-      <c r="A19" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="C19" s="19">
         <v>666</v>
@@ -1296,268 +1394,289 @@
         <v>1</v>
       </c>
       <c r="E19" s="19">
-        <f>C19*D19</f>
+        <f t="shared" si="3"/>
         <v>666</v>
       </c>
       <c r="F19" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" ht="38.5" x14ac:dyDescent="0.6">
-      <c r="A20" s="21" t="s">
+    <row r="20" spans="1:7" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A20" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="19">
+        <v>666</v>
+      </c>
+      <c r="D20" s="19">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="3"/>
+        <v>666</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.4">
+      <c r="A21" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B21" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C21" s="22">
         <v>84</v>
       </c>
-      <c r="D20" s="22">
-        <v>1</v>
-      </c>
-      <c r="E20" s="19">
-        <f>C20*D20</f>
+      <c r="D21" s="22">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19">
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F21" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A21" s="24" t="s">
+    <row r="22" spans="1:7" ht="341.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C22" s="25">
         <v>22031</v>
       </c>
-      <c r="D21" s="26">
-        <v>1</v>
-      </c>
-      <c r="E21" s="19">
-        <f>C21*D21</f>
+      <c r="D22" s="26">
+        <v>1</v>
+      </c>
+      <c r="E22" s="19">
+        <f t="shared" si="3"/>
         <v>22031</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F22" s="23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="208" x14ac:dyDescent="0.6">
-      <c r="A22" s="24" t="s">
+    <row r="23" spans="1:7" ht="183.75" x14ac:dyDescent="0.4">
+      <c r="A23" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B23" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C23" s="25">
         <v>459</v>
       </c>
-      <c r="D22" s="26">
-        <v>1</v>
-      </c>
-      <c r="E22" s="19">
-        <f>C22*D22</f>
+      <c r="D23" s="26">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19">
+        <f t="shared" si="3"/>
         <v>459</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="104" x14ac:dyDescent="0.6">
-      <c r="A23" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="25">
-        <v>234</v>
-      </c>
-      <c r="D23" s="26">
-        <v>1</v>
-      </c>
-      <c r="E23" s="27">
-        <f>C23*D23</f>
-        <v>234</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.6">
+    </row>
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.4">
       <c r="A24" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="22"/>
+        <v>56</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="C24" s="25">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="D24" s="26">
         <v>1</v>
       </c>
       <c r="E24" s="27">
-        <f>C24*D24</f>
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>234</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="78" x14ac:dyDescent="0.6">
-      <c r="A25" s="28" t="s">
+      <c r="G24" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="25">
+        <v>100</v>
+      </c>
+      <c r="D25" s="26">
+        <v>1</v>
+      </c>
+      <c r="E25" s="27">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="A26" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B26" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C26" s="30">
         <v>16445.439999999999</v>
       </c>
-      <c r="D25" s="31">
-        <v>1</v>
-      </c>
-      <c r="E25" s="32">
-        <f>C25*D25</f>
+      <c r="D26" s="31">
+        <v>1</v>
+      </c>
+      <c r="E26" s="32">
+        <f t="shared" si="3"/>
         <v>16445.439999999999</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F26" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G26" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="104" x14ac:dyDescent="0.6">
-      <c r="A26" s="35" t="s">
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.4">
+      <c r="A27" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37">
-        <f t="shared" ref="E26:E31" si="3">C26*D26</f>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="37">
+        <f t="shared" ref="E27:E32" si="4">C27*D27</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="78" x14ac:dyDescent="0.6">
-      <c r="A27" s="35" t="s">
+    <row r="28" spans="1:7" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="A28" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="38">
+      <c r="B28" s="36"/>
+      <c r="C28" s="38">
         <v>24000</v>
       </c>
-      <c r="D27" s="39">
-        <v>1</v>
-      </c>
-      <c r="E27" s="37">
-        <f t="shared" si="3"/>
+      <c r="D28" s="39">
+        <v>1</v>
+      </c>
+      <c r="E28" s="37">
+        <f t="shared" si="4"/>
         <v>24000</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A28" s="35" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="35" t="s">
         <v>69</v>
-      </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:7" ht="52" x14ac:dyDescent="0.6">
-      <c r="A29" s="35" t="s">
-        <v>70</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
       <c r="E29" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.6">
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:7" ht="52.5" x14ac:dyDescent="0.4">
       <c r="A30" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
       <c r="E30" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="156" x14ac:dyDescent="0.6">
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="157.5" x14ac:dyDescent="0.4">
+      <c r="A32" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36">
         <v>15000</v>
       </c>
-      <c r="D31" s="36">
-        <v>1</v>
-      </c>
-      <c r="E31" s="37">
-        <f t="shared" si="3"/>
+      <c r="D32" s="36">
+        <v>1</v>
+      </c>
+      <c r="E32" s="37">
+        <f t="shared" si="4"/>
         <v>15000</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A33" s="40" t="s">
+    <row r="34" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="40" t="s">
         <v>73</v>
-      </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="43">
-        <f>SUM(E2:E31)</f>
-        <v>93231.09</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="52" x14ac:dyDescent="0.6">
-      <c r="A34" s="40" t="s">
-        <v>75</v>
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="41"/>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="44">
-        <f>SUM(E2:E25)</f>
+      <c r="E34" s="43">
+        <f>SUM(E3:E32)</f>
+        <v>93231.09</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="A35" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="44">
+        <f>SUM(E3:E26)</f>
         <v>54231.09</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{67603301-8CB6-48F2-9CE2-619A3989F06E}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{C0CD1A37-61E5-49D2-9D9D-A3297CC3F027}"/>
-    <hyperlink ref="F11" r:id="rId3" xr:uid="{4F3BD2FA-4E54-458E-9A60-2B839C17449E}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{67603301-8CB6-48F2-9CE2-619A3989F06E}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{C0CD1A37-61E5-49D2-9D9D-A3297CC3F027}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{4F3BD2FA-4E54-458E-9A60-2B839C17449E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="25" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
@@ -1569,6 +1688,415 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8A43BB-496F-4BE2-91EB-BBB710B0EA64}">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="31.78515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.35546875" customWidth="1"/>
+    <col min="4" max="4" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="102.2109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="126" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="182.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="8">
+        <v>840.2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E6" si="0">C3*D3</f>
+        <v>840.2</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="110.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="8">
+        <v>153.07</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>153.07</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="110.25" x14ac:dyDescent="0.4">
+      <c r="A5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="45">
+        <v>83.25</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>83.25</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="262.5" x14ac:dyDescent="0.4">
+      <c r="A6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8">
+        <v>171.81</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>171.81</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="288.75" x14ac:dyDescent="0.4">
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43.78</v>
+      </c>
+      <c r="D7" s="13">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>146.19999999999999</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="47"/>
+    </row>
+    <row r="8" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12.96</v>
+      </c>
+      <c r="D8" s="8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" ref="E8:E9" si="1">C8*D8</f>
+        <v>77.760000000000005</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="110.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="13">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="D9" s="13">
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="1"/>
+        <v>58.679999999999993</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+    </row>
+    <row r="11" spans="1:13" ht="146.25" x14ac:dyDescent="0.4">
+      <c r="A11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13">
+        <v>72.89</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <f>C11*D11</f>
+        <v>72.89</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+    </row>
+    <row r="12" spans="1:13" ht="128.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13">
+        <v>46.75</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" ref="E12:E16" si="2">C12*D12</f>
+        <v>46.75</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="49"/>
+    </row>
+    <row r="14" spans="1:13" ht="92.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="48">
+        <v>816.88</v>
+      </c>
+      <c r="D14" s="48">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="2"/>
+        <v>816.88</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="48">
+        <v>163.4</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="2"/>
+        <v>163.4</v>
+      </c>
+      <c r="F15" s="49"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="48">
+        <v>123.5</v>
+      </c>
+      <c r="D16" s="48">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="2"/>
+        <v>123.5</v>
+      </c>
+      <c r="F16" s="49"/>
+    </row>
+    <row r="17" spans="1:6" ht="164.25" x14ac:dyDescent="0.4">
+      <c r="A17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="8">
+        <v>197.2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" ref="E17" si="3">C17*D17</f>
+        <v>394.4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="A18" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="30">
+        <v>16445.439999999999</v>
+      </c>
+      <c r="D18" s="31">
+        <v>1</v>
+      </c>
+      <c r="E18" s="32">
+        <f t="shared" ref="E18" si="4">C18*D18</f>
+        <v>16445.439999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E3:E17)</f>
+        <v>3148.7900000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f>SUM(E3:E18)</f>
+        <v>19594.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{981F3F56-14DD-46D3-B72E-B7565E20F707}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{305BA817-DF3D-4057-B669-32B2045ECA07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1576,15 +2104,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005EE9D0275751E24E9D699D551A5DF0A4" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db79dba6482692f773f90559890f60f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9e8c2109-5918-49a3-a556-c6189586690d" xmlns:ns4="431fc7b7-c7d1-4168-8930-f80b31797d45" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="752dbf6020f8ef67697a832c418e5dc4" ns3:_="" ns4:_="">
     <xsd:import namespace="9e8c2109-5918-49a3-a556-c6189586690d"/>
@@ -1769,6 +2288,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C51989C-A7D0-4414-9ECE-BEFAD571677C}">
   <ds:schemaRefs>
@@ -1779,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{568F9FFC-4950-4C53-BA08-8CEBB39234D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96020A0C-F780-4141-9D1C-CC723C36A007}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1803,4 +2323,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{568F9FFC-4950-4C53-BA08-8CEBB39234D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>